<commit_message>
Updated font in excel sheets, added test result images.
</commit_message>
<xml_diff>
--- a/data/RabbitMQ/RPC benchmarks data.xlsx
+++ b/data/RabbitMQ/RPC benchmarks data.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="RPC_Raw_Data" sheetId="1" r:id="rId1"/>
@@ -499,12 +499,12 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:shape val="box"/>
-        <c:axId val="324734720"/>
-        <c:axId val="199886176"/>
+        <c:axId val="267474560"/>
+        <c:axId val="334398480"/>
         <c:axId val="0"/>
       </c:bar3DChart>
       <c:catAx>
-        <c:axId val="324734720"/>
+        <c:axId val="267474560"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -526,7 +526,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -541,7 +541,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="199886176"/>
+        <c:crossAx val="334398480"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -549,7 +549,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="199886176"/>
+        <c:axId val="334398480"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -656,7 +656,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="324734720"/>
+        <c:crossAx val="267474560"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1648,11 +1648,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="197781600"/>
-        <c:axId val="324631536"/>
+        <c:axId val="340741696"/>
+        <c:axId val="340327344"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="197781600"/>
+        <c:axId val="340741696"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1756,7 +1756,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="324631536"/>
+        <c:crossAx val="340327344"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1764,7 +1764,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="324631536"/>
+        <c:axId val="340327344"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1876,7 +1876,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="197781600"/>
+        <c:crossAx val="340741696"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4175,8 +4175,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="S10" sqref="S10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4264,7 +4264,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:E9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+    <sheetView topLeftCell="A2" workbookViewId="0">
       <selection activeCell="W17" sqref="W17"/>
     </sheetView>
   </sheetViews>

</xml_diff>